<commit_message>
reduced constant C inputs in realistic range and converted kinetic parameters for acive uptake laws from soils
</commit_message>
<xml_diff>
--- a/test/inputs/scenario_test.xlsx
+++ b/test/inputs/scenario_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\rhizodep\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA83D93-034D-4C2F-94EC-CA0272F27985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A418DD5A-1E6E-468D-BFF2-14132494688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -2099,7 +2099,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2300,6 +2300,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="51" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2625,10 +2628,10 @@
   <dimension ref="A1:F192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B124" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H26" sqref="H26"/>
+      <selection pane="bottomRight" activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5615,10 +5618,12 @@
         <v>6.3200000000000001E-3</v>
       </c>
       <c r="E149" s="90">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="F149" s="70">
-        <v>6.3200000000000001E-3</v>
+        <f>0.0000001/2000</f>
+        <v>4.9999999999999995E-11</v>
+      </c>
+      <c r="F149" s="95">
+        <f>E149</f>
+        <v>4.9999999999999995E-11</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -5738,7 +5743,8 @@
         <v>2.0000000000000001E-9</v>
       </c>
       <c r="F155" s="55">
-        <v>3.2100000000000002E-6</v>
+        <f>E155</f>
+        <v>2.0000000000000001E-9</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -5835,10 +5841,12 @@
         <v>1.6666666666666666E-4</v>
       </c>
       <c r="E160" s="38">
-        <v>1.6666666666666666E-4</v>
+        <f>0.00016 * 100000 / 0.5</f>
+        <v>32</v>
       </c>
       <c r="F160" s="55">
-        <v>1.6666666666666666E-4</v>
+        <f>E160</f>
+        <v>32</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
proper wheat scenario, nb 142 for Rhizodep publication
</commit_message>
<xml_diff>
--- a/test/inputs/scenario_test.xlsx
+++ b/test/inputs/scenario_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\rhizodep\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A418DD5A-1E6E-468D-BFF2-14132494688E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E54D9C2-2CAB-4E79-A8E4-B45F1E5C8E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="471">
   <si>
     <t>input_file</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>sc102</t>
   </si>
 </sst>
 </file>
@@ -2628,10 +2631,10 @@
   <dimension ref="A1:F192"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B124" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G149" sqref="G149"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,8 +2659,8 @@
       <c r="D1" s="40" t="s">
         <v>382</v>
       </c>
-      <c r="E1" s="41">
-        <v>102</v>
+      <c r="E1" s="41" t="s">
+        <v>470</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>469</v>

</xml_diff>

<commit_message>
After deactivating PlantGL display in the tests
</commit_message>
<xml_diff>
--- a/test/inputs/scenario_test.xlsx
+++ b/test/inputs/scenario_test.xlsx
@@ -2703,7 +2703,7 @@
   <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
@@ -3243,7 +3243,7 @@
         <v>87</v>
       </c>
       <c r="E31" s="88" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
After moving some Python scripts in src/openalea/rhizodep/tool/
</commit_message>
<xml_diff>
--- a/test/inputs/scenario_test.xlsx
+++ b/test/inputs/scenario_test.xlsx
@@ -2703,10 +2703,10 @@
   <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3243,7 +3243,7 @@
         <v>87</v>
       </c>
       <c r="E31" s="88" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>